<commit_message>
Modelo relacional actualizado y script de creacion de tablas creado
</commit_message>
<xml_diff>
--- a/data/ModeloRelacional.xlsx
+++ b/data/ModeloRelacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/ja_avelino_uniandes_edu_co/Documents/Documentos/University/FourthSemester/Sistrans/Proyecto/EPSAndes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E71D9363-A88F-453C-9097-A335D768C10F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{E71D9363-A88F-453C-9097-A335D768C10F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5DACEA1F-24C8-4900-8DF3-B5E73989AB35}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B835AAD5-3698-49F1-B41E-42EF5DAEB5C8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
   <si>
     <t>TipoServicio</t>
   </si>
@@ -234,9 +234,6 @@
     <t>FK_TipoID.IdTipo, NN</t>
   </si>
   <si>
-    <t>NumeroID</t>
-  </si>
-  <si>
     <t>FechaNacimiento</t>
   </si>
   <si>
@@ -247,6 +244,42 @@
   </si>
   <si>
     <t>FK_Medico.IdMedico, NN</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>IdRol</t>
+  </si>
+  <si>
+    <t>IdUsuario</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>NN, CK("%@%.%")</t>
+  </si>
+  <si>
+    <t>FK_Rol.IdRol, NN</t>
+  </si>
+  <si>
+    <t>Recepcionista</t>
+  </si>
+  <si>
+    <t>IdRecepcionista</t>
+  </si>
+  <si>
+    <t>FK_Usuario.IdUsuario, NN</t>
+  </si>
+  <si>
+    <t>TrabajaEn</t>
+  </si>
+  <si>
+    <t>PK, FK_IPS.IdIPS</t>
+  </si>
+  <si>
+    <t>PK, FK_Medico.IdMedico</t>
   </si>
 </sst>
 </file>
@@ -463,12 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,9 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,6 +525,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,15 +849,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D3B51F-60FB-43F0-B98A-4B09DC3A9AF8}">
-  <dimension ref="D2:BW14"/>
+  <dimension ref="D2:BQ20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BN1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="20.77734375" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" customWidth="1"/>
     <col min="18" max="18" width="14.5546875" customWidth="1"/>
     <col min="19" max="19" width="19.109375" customWidth="1"/>
     <col min="20" max="20" width="16.5546875" customWidth="1"/>
@@ -837,36 +877,35 @@
     <col min="31" max="31" width="10.77734375" customWidth="1"/>
     <col min="33" max="33" width="17.21875" customWidth="1"/>
     <col min="34" max="34" width="14.44140625" customWidth="1"/>
-    <col min="37" max="37" width="18.21875" customWidth="1"/>
-    <col min="38" max="38" width="12" customWidth="1"/>
-    <col min="40" max="40" width="18" customWidth="1"/>
-    <col min="41" max="41" width="12.5546875" customWidth="1"/>
-    <col min="42" max="42" width="12.109375" customWidth="1"/>
-    <col min="46" max="46" width="24.21875" customWidth="1"/>
-    <col min="49" max="49" width="11.6640625" customWidth="1"/>
-    <col min="50" max="50" width="24.109375" customWidth="1"/>
-    <col min="52" max="52" width="11.77734375" customWidth="1"/>
-    <col min="53" max="53" width="10.109375" customWidth="1"/>
-    <col min="54" max="54" width="11.6640625" customWidth="1"/>
-    <col min="58" max="58" width="13.5546875" customWidth="1"/>
-    <col min="60" max="60" width="11.21875" customWidth="1"/>
-    <col min="61" max="61" width="19.44140625" customWidth="1"/>
-    <col min="64" max="64" width="10" customWidth="1"/>
-    <col min="65" max="65" width="11.44140625" customWidth="1"/>
-    <col min="66" max="66" width="19" customWidth="1"/>
-    <col min="67" max="67" width="24" customWidth="1"/>
-    <col min="68" max="68" width="19" customWidth="1"/>
-    <col min="71" max="71" width="15.88671875" customWidth="1"/>
-    <col min="74" max="74" width="15.21875" customWidth="1"/>
-    <col min="75" max="75" width="19.5546875" customWidth="1"/>
+    <col min="36" max="36" width="18.21875" customWidth="1"/>
+    <col min="37" max="37" width="12" customWidth="1"/>
+    <col min="39" max="39" width="18" customWidth="1"/>
+    <col min="40" max="40" width="12.5546875" customWidth="1"/>
+    <col min="41" max="41" width="12.109375" customWidth="1"/>
+    <col min="45" max="45" width="24.21875" customWidth="1"/>
+    <col min="48" max="48" width="11.6640625" customWidth="1"/>
+    <col min="49" max="49" width="24.109375" customWidth="1"/>
+    <col min="51" max="51" width="11.77734375" customWidth="1"/>
+    <col min="52" max="52" width="10.109375" customWidth="1"/>
+    <col min="53" max="53" width="11.6640625" customWidth="1"/>
+    <col min="56" max="56" width="13.5546875" customWidth="1"/>
+    <col min="57" max="57" width="11.21875" customWidth="1"/>
+    <col min="58" max="58" width="19.44140625" customWidth="1"/>
+    <col min="61" max="61" width="10" customWidth="1"/>
+    <col min="62" max="62" width="11.44140625" customWidth="1"/>
+    <col min="63" max="63" width="19" customWidth="1"/>
+    <col min="64" max="64" width="24" customWidth="1"/>
+    <col min="65" max="65" width="19" customWidth="1"/>
+    <col min="68" max="68" width="15.21875" customWidth="1"/>
+    <col min="69" max="69" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:69" x14ac:dyDescent="0.3">
       <c r="L2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="AJ2" s="1"/>
+      <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:69" x14ac:dyDescent="0.3">
       <c r="F3" s="1"/>
       <c r="I3" s="1"/>
       <c r="L3" s="1"/>
@@ -874,13 +913,13 @@
       <c r="W3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="BC3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="BB3" s="1"/>
     </row>
-    <row r="4" spans="4:75" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F4" s="1"/>
       <c r="I4" s="1"/>
       <c r="L4" s="1"/>
@@ -888,155 +927,149 @@
       <c r="W4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AF4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="BC4" s="1"/>
-      <c r="BJ4" s="1"/>
-      <c r="BQ4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="BB4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="BN4" s="1"/>
     </row>
-    <row r="5" spans="4:75" x14ac:dyDescent="0.3">
-      <c r="D5" s="6" t="s">
+    <row r="5" spans="4:69" x14ac:dyDescent="0.3">
+      <c r="D5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="18"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="7"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="18"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="7"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="18"/>
       <c r="W5" s="2"/>
-      <c r="X5" s="6" t="s">
+      <c r="X5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="7"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="18"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="6" t="s">
+      <c r="AD5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AE5" s="7"/>
+      <c r="AE5" s="18"/>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="6" t="s">
+      <c r="AG5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="6" t="s">
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="2"/>
-      <c r="AN5" s="6" t="s">
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="7"/>
-      <c r="AQ5" s="2"/>
-      <c r="AR5" s="6" t="s">
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="7"/>
-      <c r="AU5" s="2"/>
-      <c r="AV5" s="6" t="s">
+      <c r="AR5" s="17"/>
+      <c r="AS5" s="18"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="14"/>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="14"/>
-      <c r="BA5" s="14"/>
-      <c r="BB5" s="7"/>
-      <c r="BC5" s="2"/>
-      <c r="BD5" s="6" t="s">
+      <c r="AV5" s="17"/>
+      <c r="AW5" s="17"/>
+      <c r="AX5" s="17"/>
+      <c r="AY5" s="17"/>
+      <c r="AZ5" s="17"/>
+      <c r="BA5" s="18"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="BE5" s="14"/>
-      <c r="BF5" s="14"/>
-      <c r="BG5" s="14"/>
-      <c r="BH5" s="14"/>
-      <c r="BI5" s="7"/>
-      <c r="BJ5" s="2"/>
-      <c r="BK5" s="6" t="s">
+      <c r="BD5" s="17"/>
+      <c r="BE5" s="17"/>
+      <c r="BF5" s="18"/>
+      <c r="BG5" s="2"/>
+      <c r="BH5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="BL5" s="14"/>
-      <c r="BM5" s="14"/>
-      <c r="BN5" s="14"/>
-      <c r="BO5" s="14"/>
-      <c r="BP5" s="7"/>
-      <c r="BQ5" s="2"/>
-      <c r="BR5" s="6" t="s">
+      <c r="BI5" s="17"/>
+      <c r="BJ5" s="17"/>
+      <c r="BK5" s="17"/>
+      <c r="BL5" s="17"/>
+      <c r="BM5" s="18"/>
+      <c r="BN5" s="2"/>
+      <c r="BO5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="BS5" s="14"/>
-      <c r="BT5" s="14"/>
-      <c r="BU5" s="14"/>
-      <c r="BV5" s="14"/>
-      <c r="BW5" s="7"/>
+      <c r="BP5" s="17"/>
+      <c r="BQ5" s="18"/>
     </row>
-    <row r="6" spans="4:75" x14ac:dyDescent="0.3">
-      <c r="D6" s="8" t="s">
+    <row r="6" spans="4:69" x14ac:dyDescent="0.3">
+      <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>12</v>
@@ -1047,11 +1080,11 @@
       <c r="U6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="V6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="W6" s="3"/>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Y6" s="4" t="s">
@@ -1063,166 +1096,148 @@
       <c r="AA6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AB6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="AC6" s="3"/>
-      <c r="AD6" s="8" t="s">
+      <c r="AD6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AE6" s="9" t="s">
+      <c r="AE6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="AF6" s="3"/>
-      <c r="AG6" s="8" t="s">
+      <c r="AG6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AH6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI6" s="9" t="s">
+      <c r="AH6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU6" s="3"/>
-      <c r="AV6" s="8" t="s">
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="AV6" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="AW6" s="4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="AX6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="BI6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="BJ6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BL6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AY6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC6" s="3"/>
-      <c r="BD6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="BF6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BG6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BH6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI6" s="9" t="s">
+      <c r="BM6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN6" s="3"/>
+      <c r="BO6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BJ6" s="3"/>
-      <c r="BK6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="BL6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="BM6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="BN6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="BO6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="BP6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="BQ6" s="3"/>
-      <c r="BR6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="BS6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="BT6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BV6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BW6" s="9" t="s">
-        <v>60</v>
-      </c>
     </row>
-    <row r="7" spans="4:75" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="11" t="s">
+    <row r="7" spans="4:69" x14ac:dyDescent="0.3">
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="11" t="s">
+      <c r="G7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="J7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="R7" s="5" t="s">
@@ -1237,11 +1252,11 @@
       <c r="U7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V7" s="11" t="s">
+      <c r="V7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="W7" s="3"/>
-      <c r="X7" s="10" t="s">
+      <c r="X7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="Y7" s="5" t="s">
@@ -1253,324 +1268,288 @@
       <c r="AA7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AB7" s="11" t="s">
+      <c r="AB7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE7" s="11" t="s">
+      <c r="AD7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="AF7" s="3"/>
-      <c r="AG7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI7" s="11" t="s">
+      <c r="AG7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL7" s="11" t="s">
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO7" s="5" t="s">
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AP7" s="11" t="s">
+      <c r="BA7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU7" s="3"/>
-      <c r="AV7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AW7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AZ7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BA7" s="5" t="s">
+      <c r="BF7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BI7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="BB7" s="11" t="s">
+      <c r="BJ7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BK7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BL7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BN7" s="3"/>
+      <c r="BO7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BP7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="BC7" s="3"/>
-      <c r="BD7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="BE7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BF7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BG7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="BH7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="BI7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="BJ7" s="3"/>
-      <c r="BK7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="BL7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="BM7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BN7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BO7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BP7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="BQ7" s="3"/>
-      <c r="BR7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="BS7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BT7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="BU7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="BV7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="BW7" s="11" t="s">
+      <c r="BQ7" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="4:75" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="12" t="s">
+    <row r="8" spans="4:69" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="15" t="s">
+      <c r="R8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="T8" s="16" t="s">
+      <c r="T8" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U8" s="15" t="s">
+      <c r="U8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="V8" s="13" t="s">
+      <c r="V8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="W8" s="3"/>
-      <c r="X8" s="17" t="s">
+      <c r="X8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="Y8" s="15" t="s">
+      <c r="Y8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Z8" s="15" t="s">
+      <c r="Z8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AA8" s="15" t="s">
+      <c r="AA8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AB8" s="18" t="s">
+      <c r="AB8" s="15" t="s">
         <v>37</v>
       </c>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="17" t="s">
+      <c r="AD8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AE8" s="13" t="s">
+      <c r="AE8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="AF8" s="3"/>
-      <c r="AG8" s="17" t="s">
+      <c r="AG8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AH8" s="15" t="s">
+      <c r="AH8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AI8" s="13" t="s">
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="17" t="s">
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AL8" s="13" t="s">
+      <c r="AN8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO8" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP8" s="13" t="s">
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT8" s="3"/>
+      <c r="AU8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AV8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AQ8" s="3"/>
-      <c r="AR8" s="12" t="s">
+      <c r="AY8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="BB8" s="3"/>
+      <c r="BC8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AS8" s="15" t="s">
+      <c r="BD8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AT8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU8" s="3"/>
-      <c r="AV8" s="12" t="s">
+      <c r="BE8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="BF8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AW8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="AX8" s="16" t="s">
+      <c r="BI8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="BJ8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK8" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AY8" s="15" t="s">
+      <c r="BM8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="BN8" s="3"/>
+      <c r="BO8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="BP8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AZ8" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BB8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="BC8" s="3"/>
-      <c r="BD8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="BE8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="BG8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BH8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BI8" s="18" t="s">
+      <c r="BQ8" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="BJ8" s="3"/>
-      <c r="BK8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="BL8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BM8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN8" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO8" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="BP8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="BQ8" s="3"/>
-      <c r="BR8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="BS8" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="BU8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BV8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BW8" s="18" t="s">
-        <v>61</v>
-      </c>
     </row>
-    <row r="9" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F9" s="1"/>
       <c r="I9" s="1"/>
       <c r="L9" s="1"/>
@@ -1578,90 +1557,256 @@
       <c r="W9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AF9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AM9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="BC9" s="1"/>
-      <c r="BJ9" s="1"/>
-      <c r="BQ9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BN9" s="1"/>
     </row>
-    <row r="10" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:69" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F10" s="1"/>
       <c r="I10" s="1"/>
       <c r="L10" s="1"/>
+      <c r="M10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18"/>
       <c r="P10" s="1"/>
       <c r="W10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AF10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AM10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AU10" s="1"/>
-      <c r="BC10" s="1"/>
-      <c r="BJ10" s="1"/>
-      <c r="BQ10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BN10" s="1"/>
     </row>
-    <row r="11" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:69" x14ac:dyDescent="0.3">
+      <c r="D11" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="18"/>
       <c r="F11" s="1"/>
       <c r="I11" s="1"/>
+      <c r="J11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="18"/>
       <c r="L11" s="1"/>
+      <c r="M11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="P11" s="1"/>
       <c r="W11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AF11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AM11" s="1"/>
-      <c r="AQ11" s="1"/>
-      <c r="AU11" s="1"/>
-      <c r="BC11" s="1"/>
-      <c r="BQ11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BN11" s="1"/>
     </row>
-    <row r="12" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:69" x14ac:dyDescent="0.3">
+      <c r="D12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="I12" s="1"/>
+      <c r="J12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="L12" s="1"/>
+      <c r="M12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="W12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AF12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AM12" s="1"/>
-      <c r="AQ12" s="1"/>
-      <c r="BC12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="BB12" s="1"/>
     </row>
-    <row r="13" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:69" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="L13" s="1"/>
+      <c r="M13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="AC13" s="1"/>
-      <c r="AM13" s="1"/>
-      <c r="BC13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="BB13" s="1"/>
     </row>
-    <row r="14" spans="4:75" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:69" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="AC14" s="1"/>
     </row>
+    <row r="16" spans="4:69" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="AV5:BB5"/>
-    <mergeCell ref="BD5:BI5"/>
-    <mergeCell ref="BK5:BP5"/>
-    <mergeCell ref="BR5:BW5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AG5:AI5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AR5:AT5"/>
+  <mergeCells count="19">
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M10:O10"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="Q5:V5"/>
-    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="AU5:BA5"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="BH5:BM5"/>
+    <mergeCell ref="BO5:BQ5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AM5:AO5"/>
+    <mergeCell ref="AQ5:AS5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010025AAF09EF7B4444D877C75BB24AC0A71" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="57464b8cca4840d710731cc5ceb7c706">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21bcf045-db39-47ec-9a7d-c59e900bf401" xmlns:ns4="e4f630af-6f71-40bf-8f35-494241594c5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46816f5ba28575ef80268cc1b4a811da" ns3:_="" ns4:_="">
     <xsd:import namespace="21bcf045-db39-47ec-9a7d-c59e900bf401"/>
@@ -1878,22 +2023,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6EA7CD-8942-4727-A0EE-A15FB4BB1F8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e4f630af-6f71-40bf-8f35-494241594c5b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="21bcf045-db39-47ec-9a7d-c59e900bf401"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D459BD82-6BEE-4DD3-A3FD-9C981097F03A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E50A606E-9B52-45D3-B91C-CFA845A23368}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1910,29 +2065,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D459BD82-6BEE-4DD3-A3FD-9C981097F03A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE6EA7CD-8942-4727-A0EE-A15FB4BB1F8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e4f630af-6f71-40bf-8f35-494241594c5b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="21bcf045-db39-47ec-9a7d-c59e900bf401"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>